<commit_message>
Changes in MSL Automation For warehouse #CRM-2719
Price column is not clear - is it basic price or total price?
GST number -> GST rate
If consumption in 30 days is 0 and current stock is 0 but consumption in
45 days is > 0, then recommended should use 45 days. U can divide 45
days in 2 and use that as recommended quantity.
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/msl_data.xlsx
+++ b/application/controllers/excel-templates/msl_data.xlsx
@@ -25,10 +25,10 @@
     <t>Part Type</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>GST Number</t>
+    <t>Basic Price</t>
+  </si>
+  <si>
+    <t>GST Rate</t>
   </si>
   <si>
     <t>Current Stock</t>

</xml_diff>